<commit_message>
adding images for sites
</commit_message>
<xml_diff>
--- a/_data/religion-rss.xlsx
+++ b/_data/religion-rss.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adbrett/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adbrett/Documents/GitHub/orange76xyz/_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{815ABB4E-DFAC-3E44-9CA8-DC9E2A0D7CB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4FEE5FA-102A-2542-853C-21DA928FE6CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{D991FF9C-148D-9342-B715-49325516D119}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="251">
   <si>
     <t>Name</t>
   </si>
@@ -98,9 +98,6 @@
     <t>https://religion.ua.edu/blog/feed/</t>
   </si>
   <si>
-    <t>https://religion.ua.edu/wp-content/uploads/2022/10/rs-logo.png</t>
-  </si>
-  <si>
     <t>https://religion.ua.edu/blog/</t>
   </si>
   <si>
@@ -125,9 +122,6 @@
     <t>https://www.whitetoolong.net/feed</t>
   </si>
   <si>
-    <t>https://substackcdn.com/image/fetch/w_96,c_limit,f_auto,q_auto:good,fl_progressive:steep/https%3A%2F%2Fbucketeer-e05bbc84-baa3-437e-9518-adb32be77984.s3.amazonaws.com%2Fpublic%2Fimages%2F6ce1d537-6962-4db0-af13-1a90653eb347_512x512.png</t>
-  </si>
-  <si>
     <t>https://anchor.fm/s/baa65a08/podcast/rss</t>
   </si>
   <si>
@@ -191,9 +185,6 @@
     <t>Te Ture Tāhae Whenua - The Doctrine of Discovery in Aotearoa</t>
   </si>
   <si>
-    <t>https://substackcdn.com/image/fetch/w_96,c_limit,f_auto,q_auto:good,fl_progressive:steep/https%3A%2F%2Fsubstack-post-media.s3.amazonaws.com%2Fpublic%2Fimages%2F8447cf58-f9d0-4a3f-a448-8f396c0a4ed9_404x404.png</t>
-  </si>
-  <si>
     <t>https://tinangata.substack.com/feed</t>
   </si>
   <si>
@@ -206,9 +197,6 @@
     <t>https://stevennewcomb.substack.com/feed/</t>
   </si>
   <si>
-    <t>https://substackcdn.com/image/fetch/w_96,c_limit,f_auto,q_auto:good,fl_progressive:steep/https%3A%2F%2Fsubstack-post-media.s3.amazonaws.com%2Fpublic%2Fimages%2F75732069-1048-4cf4-a63a-0e30714fef69_562x562.png</t>
-  </si>
-  <si>
     <t>Religion in United States History</t>
   </si>
   <si>
@@ -218,9 +206,6 @@
     <t>https://usreligion.substack.com/feed/</t>
   </si>
   <si>
-    <t>https://substackcdn.com/image/fetch/w_96,c_limit,f_auto,q_auto:good,fl_progressive:steep/https%3A%2F%2Fsubstack-post-media.s3.amazonaws.com%2Fpublic%2Fimages%2F9ff81c51-d8a9-46df-81e2-c1507960132e_144x144.png</t>
-  </si>
-  <si>
     <t>Andrew Whitehead</t>
   </si>
   <si>
@@ -278,9 +263,6 @@
     <t>https://anchor.fm/s/5e43bc9c/podcast/rss</t>
   </si>
   <si>
-    <t>https://cdn-images-3.listennotes.com/podcasts/ancient-afterlives-ancient-afterlives-yF-g3ObvNKh-LRj6ZBdJEMe.300x300.jpg</t>
-  </si>
-  <si>
     <t>Religion for Breakfast</t>
   </si>
   <si>
@@ -395,9 +377,6 @@
     <t>https://feeds.megaphone.fm/ADL4119301527</t>
   </si>
   <si>
-    <t>https://syndicate.network/wp-content/themes/kauaicreative.com/images/Syndicatenetwork_logo.svg</t>
-  </si>
-  <si>
     <t>Syndicate Network</t>
   </si>
   <si>
@@ -449,9 +428,6 @@
     <t>American Idols</t>
   </si>
   <si>
-    <t>https://cdn-images-3.listennotes.com/podcasts/american-idols-axis-mundi-media-5esWonDiBTA-puElqGJHOtf.300x300.jpg</t>
-  </si>
-  <si>
     <t>https://redcircle.com/shows/americanidols?utm_source=listennotes.com&amp;utm_campaign=Listen+Notes&amp;utm_medium=website</t>
   </si>
   <si>
@@ -485,9 +461,6 @@
     <t>https://www.wabashcenter.wabash.edu/resources/blog/</t>
   </si>
   <si>
-    <t>https://www.wabashcenter.wabash.edu/wp-content/themes/wabash-child-theme/images/logo.png</t>
-  </si>
-  <si>
     <t>https://www.wabashcenter.wabash.edu/feed/</t>
   </si>
   <si>
@@ -497,9 +470,6 @@
     <t>https://rsn.aarweb.org/</t>
   </si>
   <si>
-    <t>https://rsn.aarweb.org/sites/default/files/Religious_Studies_News_h100.png</t>
-  </si>
-  <si>
     <t>https://rsn.aarweb.org/rss.xml</t>
   </si>
   <si>
@@ -569,15 +539,9 @@
     <t>https://religiondispatches.org/</t>
   </si>
   <si>
-    <t>https://religiondispatches.org/wp-content/uploads/2014/06/rdwhatsup_crop_small.jpg</t>
-  </si>
-  <si>
     <t>https://religiondispatches.org/feed/</t>
   </si>
   <si>
-    <t>https://religionlab.virginia.edu/wp-content/uploads/2019/01/Religion_Race__Dem@2x.png</t>
-  </si>
-  <si>
     <t>Religion Race and Democracy Lab, UVA</t>
   </si>
   <si>
@@ -608,9 +572,6 @@
     <t>https://usreligion.blogspot.com/feeds/posts/default</t>
   </si>
   <si>
-    <t>https://scontent-atl3-2.xx.fbcdn.net/v/t39.30808-6/305772201_955348428689346_3707735780192118610_n.jpg?_nc_cat=105&amp;ccb=1-7&amp;_nc_sid=5f2048&amp;_nc_ohc=g-lcMKisU-MAb7ZwAu4&amp;_nc_ht=scontent-atl3-2.xx&amp;oh=00_AfBAmH9_Blz8bSgDJpY3PhUEIDnH5LX783_wEoZtwWA1eg&amp;oe=6632DB6A</t>
-  </si>
-  <si>
     <t>Religion and Politics</t>
   </si>
   <si>
@@ -620,9 +581,6 @@
     <t>https://religionandpolitics.org/feed/</t>
   </si>
   <si>
-    <t>https://religionandpolitics.org/wp-content/uploads/2023/05/Untitled-design-199.jpg</t>
-  </si>
-  <si>
     <t>Feminism and Religion</t>
   </si>
   <si>
@@ -659,15 +617,9 @@
     <t>https://www.aprilonline.org/the-commons/</t>
   </si>
   <si>
-    <t>https://www.aprilonline.org/wp-content/uploads/2020/10/April-logo02.png</t>
-  </si>
-  <si>
     <t>https://www.aprilonline.org/feed/</t>
   </si>
   <si>
-    <t>https://ssrc-static.s3.amazonaws.com/wp-content/uploads/2017/07/29175006/TIF_logo_Final-01-1.png</t>
-  </si>
-  <si>
     <t>The Immanent Frame</t>
   </si>
   <si>
@@ -704,12 +656,6 @@
     <t>https://www.patheos.com/blogs/religionprof/feed</t>
   </si>
   <si>
-    <t>https://www.patheos.com/blogs/wp-content/themes/Patheos%20TwentySeventeen/assets/images/favicons/apple-touch-icon.png</t>
-  </si>
-  <si>
-    <t>https://religionmatters.org/wp-content/uploads/2023/04/cropped-Original-Logo-1.png?w=2021&amp;ssl=1</t>
-  </si>
-  <si>
     <t>Jewish Philosophy Place</t>
   </si>
   <si>
@@ -783,6 +729,66 @@
   </si>
   <si>
     <t>politicaltheology.png</t>
+  </si>
+  <si>
+    <t>religionandpolitics.jpg</t>
+  </si>
+  <si>
+    <t>religiondispatches.jpg</t>
+  </si>
+  <si>
+    <t>usreligion.jpg</t>
+  </si>
+  <si>
+    <t>religioninunitedstateshistory.jpg</t>
+  </si>
+  <si>
+    <t>religionmatters.png</t>
+  </si>
+  <si>
+    <t>religionlab.png</t>
+  </si>
+  <si>
+    <t>patheos.png</t>
+  </si>
+  <si>
+    <t>rsn.png</t>
+  </si>
+  <si>
+    <t>religiousstudiesproject.png</t>
+  </si>
+  <si>
+    <t>religion-ua.png</t>
+  </si>
+  <si>
+    <t>Syndicatenetwork.svg</t>
+  </si>
+  <si>
+    <t>tinangata.jpg</t>
+  </si>
+  <si>
+    <t>aprilonline.png</t>
+  </si>
+  <si>
+    <t>stevennewcomb.jpg</t>
+  </si>
+  <si>
+    <t>the-immanent-frame.png</t>
+  </si>
+  <si>
+    <t>the-revealer.png</t>
+  </si>
+  <si>
+    <t>wabash.png</t>
+  </si>
+  <si>
+    <t>whitetoolong.jpg</t>
+  </si>
+  <si>
+    <t>american-idols.jpg</t>
+  </si>
+  <si>
+    <t>ancient-afterlives.jpg</t>
   </si>
 </sst>
 </file>
@@ -847,7 +853,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -859,6 +865,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1197,12 +1204,13 @@
   <dimension ref="A1:E63"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C21" sqref="C21"/>
+      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="33.5" customWidth="1"/>
     <col min="3" max="3" width="32" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1225,121 +1233,121 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>227</v>
+        <v>209</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>226</v>
+        <v>208</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>229</v>
+        <v>211</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>228</v>
+        <v>210</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>230</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>45</v>
-      </c>
       <c r="E3" s="3" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>231</v>
+        <v>213</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>232</v>
+        <v>214</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>233</v>
+        <v>215</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>170</v>
+        <v>160</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="B7" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>234</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>123</v>
-      </c>
       <c r="E7" s="3" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>244</v>
+        <v>226</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -1350,27 +1358,27 @@
         <v>13</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>236</v>
+        <v>218</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>11</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>237</v>
+        <v>219</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>10</v>
@@ -1378,308 +1386,308 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="D11" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B11" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>238</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>39</v>
-      </c>
       <c r="E11" s="3" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>195</v>
+        <v>181</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>196</v>
+        <v>182</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>239</v>
+        <v>221</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>197</v>
+        <v>183</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>240</v>
+        <v>222</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="D14" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B14" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>241</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>42</v>
-      </c>
       <c r="E14" s="3" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="C15" s="3" t="s">
         <v>224</v>
       </c>
-      <c r="B15" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>242</v>
-      </c>
       <c r="D15" s="3" t="s">
-        <v>225</v>
+        <v>207</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>243</v>
+        <v>225</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>155</v>
+        <v>145</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>156</v>
+        <v>146</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>245</v>
+        <v>227</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>213</v>
+        <v>197</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>214</v>
+        <v>198</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>246</v>
+        <v>228</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>215</v>
+        <v>199</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="D19" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="B19" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>247</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>48</v>
-      </c>
       <c r="E19" s="3" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>248</v>
+        <v>230</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
-        <v>191</v>
+        <v>178</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>192</v>
+        <v>179</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>194</v>
+        <v>231</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>193</v>
+        <v>180</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
-        <v>175</v>
+        <v>165</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>177</v>
+        <v>232</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>178</v>
+        <v>167</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
-        <v>187</v>
+        <v>175</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>188</v>
+        <v>176</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>190</v>
+        <v>233</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>189</v>
+        <v>177</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>60</v>
+        <v>234</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
-        <v>216</v>
+        <v>200</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>217</v>
+        <v>201</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>223</v>
+        <v>235</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>218</v>
+        <v>202</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
-        <v>180</v>
+        <v>168</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>181</v>
+        <v>169</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>179</v>
+        <v>236</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
-        <v>219</v>
+        <v>203</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>220</v>
+        <v>204</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>222</v>
+        <v>237</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>221</v>
+        <v>205</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>153</v>
+        <v>238</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>154</v>
+        <v>144</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
@@ -1690,13 +1698,13 @@
         <v>7</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>8</v>
+        <v>239</v>
       </c>
       <c r="D29" s="3" t="s">
         <v>6</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
@@ -1704,166 +1712,166 @@
         <v>18</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>20</v>
+        <v>240</v>
       </c>
       <c r="D30" s="3" t="s">
         <v>19</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>119</v>
+        <v>241</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B32" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="D32" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="C32" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="D32" s="3" t="s">
-        <v>52</v>
-      </c>
       <c r="E32" s="3" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
-        <v>205</v>
+        <v>191</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>206</v>
+        <v>192</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>207</v>
+        <v>243</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>208</v>
+        <v>193</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>54</v>
+        <v>50</v>
+      </c>
+      <c r="B34" s="7" t="s">
+        <v>51</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>56</v>
+        <v>244</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
-        <v>210</v>
+        <v>194</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>211</v>
+        <v>195</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>209</v>
+        <v>245</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>212</v>
+        <v>196</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="C36" s="3" t="s">
-        <v>161</v>
+        <v>149</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>246</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>160</v>
+        <v>150</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>149</v>
+        <v>247</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B38" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B38" s="3" t="s">
+      <c r="C38" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="D38" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C38" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D38" s="5" t="s">
-        <v>28</v>
-      </c>
       <c r="E38" s="3" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>137</v>
+        <v>249</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="E39" s="3" t="s">
         <v>10</v>
@@ -1871,16 +1879,16 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>80</v>
+        <v>250</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="E40" s="3" t="s">
         <v>10</v>
@@ -1888,16 +1896,16 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="E41" s="3" t="s">
         <v>10</v>
@@ -1905,16 +1913,16 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="E42" s="3" t="s">
         <v>10</v>
@@ -1922,16 +1930,16 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="E43" s="3" t="s">
         <v>10</v>
@@ -1939,16 +1947,16 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="E44" s="3" t="s">
         <v>10</v>
@@ -1956,16 +1964,16 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="E45" s="3" t="s">
         <v>10</v>
@@ -1973,16 +1981,16 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="E46" s="3" t="s">
         <v>10</v>
@@ -1990,16 +1998,16 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="E47" s="3" t="s">
         <v>10</v>
@@ -2007,16 +2015,16 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C48" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B48" s="3" t="s">
+      <c r="D48" s="3" t="s">
         <v>34</v>
-      </c>
-      <c r="C48" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D48" s="3" t="s">
-        <v>36</v>
       </c>
       <c r="E48" s="3" t="s">
         <v>10</v>
@@ -2024,14 +2032,14 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
-        <v>198</v>
+        <v>184</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>199</v>
+        <v>185</v>
       </c>
       <c r="C49" s="3"/>
       <c r="D49" s="3" t="s">
-        <v>200</v>
+        <v>186</v>
       </c>
       <c r="E49" s="3" t="s">
         <v>10</v>
@@ -2039,16 +2047,16 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="E50" s="3" t="s">
         <v>10</v>
@@ -2056,16 +2064,16 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="E51" s="3" t="s">
         <v>10</v>
@@ -2073,16 +2081,16 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="s">
-        <v>201</v>
+        <v>187</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>203</v>
+        <v>189</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>204</v>
+        <v>190</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>202</v>
+        <v>188</v>
       </c>
       <c r="E52" s="3" t="s">
         <v>10</v>
@@ -2090,16 +2098,16 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" s="3" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="E53" s="3" t="s">
         <v>10</v>
@@ -2107,16 +2115,16 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" s="3" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="E54" s="3" t="s">
         <v>10</v>
@@ -2124,16 +2132,16 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" s="3" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="E55" s="3" t="s">
         <v>10</v>
@@ -2141,16 +2149,16 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B56" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D56" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="C56" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D56" s="3" t="s">
-        <v>24</v>
       </c>
       <c r="E56" s="3" t="s">
         <v>10</v>
@@ -2175,16 +2183,16 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" s="3" t="s">
-        <v>183</v>
+        <v>171</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>184</v>
+        <v>172</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>186</v>
+        <v>174</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>185</v>
+        <v>173</v>
       </c>
       <c r="E58" s="3" t="s">
         <v>10</v>
@@ -2192,16 +2200,16 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" s="3" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="E59" s="3" t="s">
         <v>10</v>
@@ -2226,16 +2234,16 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" s="3" t="s">
-        <v>162</v>
+        <v>152</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>163</v>
+        <v>153</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>161</v>
+        <v>151</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="E61" s="3" t="s">
         <v>10</v>
@@ -2243,16 +2251,16 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" s="3" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="E62" s="3" t="s">
         <v>10</v>
@@ -2260,16 +2268,16 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" s="3" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>235</v>
+        <v>217</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="E63" s="3" t="s">
         <v>10</v>
@@ -2290,13 +2298,13 @@
     <hyperlink ref="D5" r:id="rId7" xr:uid="{834AD146-D3D9-A941-86A7-9884124E7D31}"/>
     <hyperlink ref="D4" r:id="rId8" xr:uid="{7551C065-674E-5743-B511-DD2FC8C49589}"/>
     <hyperlink ref="B20" r:id="rId9" xr:uid="{F9A7199E-1CD1-9942-8713-D32FAAA9E11C}"/>
-    <hyperlink ref="C25" r:id="rId10" xr:uid="{416D265A-81BE-E643-8D3A-B57D61C2BDD0}"/>
-    <hyperlink ref="D2" r:id="rId11" xr:uid="{EFB4000A-3FFE-9A43-B1D8-627B49450530}"/>
-    <hyperlink ref="B5" r:id="rId12" xr:uid="{B94C9833-A875-4B43-BA9C-B43DF2CB8472}"/>
-    <hyperlink ref="B6" r:id="rId13" xr:uid="{D8DE5E70-A924-F54C-BB9B-33961DB9D429}"/>
-    <hyperlink ref="B12" r:id="rId14" xr:uid="{ED624B05-2FB0-214E-BAD0-60FD81F31905}"/>
-    <hyperlink ref="B15" r:id="rId15" xr:uid="{53E58936-2425-B24B-9995-38458968360E}"/>
-    <hyperlink ref="B16" r:id="rId16" xr:uid="{2B9B0FFB-DD46-4A48-9395-77518F1F8B40}"/>
+    <hyperlink ref="D2" r:id="rId10" xr:uid="{EFB4000A-3FFE-9A43-B1D8-627B49450530}"/>
+    <hyperlink ref="B5" r:id="rId11" xr:uid="{B94C9833-A875-4B43-BA9C-B43DF2CB8472}"/>
+    <hyperlink ref="B6" r:id="rId12" xr:uid="{D8DE5E70-A924-F54C-BB9B-33961DB9D429}"/>
+    <hyperlink ref="B12" r:id="rId13" xr:uid="{ED624B05-2FB0-214E-BAD0-60FD81F31905}"/>
+    <hyperlink ref="B15" r:id="rId14" xr:uid="{53E58936-2425-B24B-9995-38458968360E}"/>
+    <hyperlink ref="B16" r:id="rId15" xr:uid="{2B9B0FFB-DD46-4A48-9395-77518F1F8B40}"/>
+    <hyperlink ref="B34" r:id="rId16" xr:uid="{3D275AAE-781B-E44D-A32D-8C30E3E3E57F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>